<commit_message>
Update User Stories.xlsx with latest changes
</commit_message>
<xml_diff>
--- a/User-Stories/User Stories.xlsx
+++ b/User-Stories/User Stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\SafePath\User-Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BD2D25-4BAD-4033-B66F-51C7CB210554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E956F0-8730-48CD-9B82-EAE7E7E1D7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43BAFF81-32F0-934D-BBDE-E19BC4484916}"/>
   </bookViews>
@@ -227,9 +227,6 @@
     <t>Urban Planner</t>
   </si>
   <si>
-    <t>Example: A transport authority in New York evaluating whether SafePath data supports cycling policy expansion.</t>
-  </si>
-  <si>
     <t>Individual users who walk or cycle in cities (students, workers, residents).</t>
   </si>
   <si>
@@ -246,6 +243,9 @@
   </si>
   <si>
     <t>Broader role than city planner - focuses on long-term urban design, transport policies, and global scaling.</t>
+  </si>
+  <si>
+    <t>Example: The transport authority evaluating whether SafePath data supports cycling policy expansion.</t>
   </si>
 </sst>
 </file>
@@ -664,10 +664,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,7 +985,7 @@
   <dimension ref="B1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -999,14 +999,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="61.95" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
@@ -1304,13 +1304,13 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
@@ -1319,13 +1319,13 @@
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="21" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
@@ -1334,13 +1334,13 @@
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
@@ -1349,33 +1349,33 @@
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="22" t="s">
+      <c r="C41" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>